<commit_message>
Clean up before next analysis.
</commit_message>
<xml_diff>
--- a/data/20190324_condition_mapper.xlsx
+++ b/data/20190324_condition_mapper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simontuke/Dropbox/TSH_2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EEBDBE-236E-2E49-AC6A-4FA09708C31D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DDF21E-16C7-234F-A0D7-ED8BF987B2AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18960" xr2:uid="{27564C4E-771A-D34D-957E-8F7EEA76391D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27020" windowHeight="26080" xr2:uid="{27564C4E-771A-D34D-957E-8F7EEA76391D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,10 +548,14 @@
   <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>